<commit_message>
Incorporate addenda a, b, and c.
</commit_message>
<xml_diff>
--- a/assets/examples/xlsx/RS0001/ASHRAE90-1-2019-bd-Curve-Set-AA.RS0001.a205.xlsx
+++ b/assets/examples/xlsx/RS0001/ASHRAE90-1-2019-bd-Curve-Set-AA.RS0001.a205.xlsx
@@ -12,6 +12,8 @@
     <sheet name="liquid_components0" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="performance_map_cooling" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="performance_map_standby" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="performance_map_evaporator_liqu" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="performance_map_condenser_liqui" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -349,22 +351,42 @@
     </comment>
     <comment ref="B29" authorId="0" shapeId="0">
       <text>
-        <t>Maximum input power at which the chiller operates reliably and continuously</t>
-      </text>
-    </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
-      <text>
         <t>Cycling degradation coefficient (C~D~) as described in AHRI 550/590 or AHRI 551/591</t>
       </text>
     </comment>
+    <comment ref="A30" authorId="0" shapeId="0">
+      <text>
+        <t>Data group describing cooling performance over a range of conditions</t>
+      </text>
+    </comment>
     <comment ref="A31" authorId="0" shapeId="0">
       <text>
-        <t>Data group describing cooling performance over a range of conditions</t>
+        <t>Data group describing standby performance</t>
       </text>
     </comment>
     <comment ref="A32" authorId="0" shapeId="0">
       <text>
-        <t>Data group describing standby performance</t>
+        <t>Data group describing the liquid pressure differential through the evaporator</t>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="0" shapeId="0">
+      <text>
+        <t>Data group describing the liquid pressure differential through the condenser</t>
+      </text>
+    </comment>
+    <comment ref="A34" authorId="0" shapeId="0">
+      <text>
+        <t>Specifies the range the performance data can be scaled to represent different capacity equipment</t>
+      </text>
+    </comment>
+    <comment ref="B35" authorId="0" shapeId="0">
+      <text>
+        <t>Minimum scaling factor</t>
+      </text>
+    </comment>
+    <comment ref="B36" authorId="0" shapeId="0">
+      <text>
+        <t>Maximum scaling factor</t>
       </text>
     </comment>
   </commentList>
@@ -469,32 +491,17 @@
     </comment>
     <comment ref="I3" authorId="0" shapeId="0">
       <text>
-        <t>Entering evaporator liquid temperature</t>
+        <t>Heat transferred to another liquid crossing the control volume boundary from the chiller oil cooler.</t>
       </text>
     </comment>
     <comment ref="J3" authorId="0" shapeId="0">
       <text>
-        <t>Leaving condenser liquid temperature</t>
+        <t>Heat transferred to another liquid crossing the control volume boundary from the chiller auxiliaries (motor, motor controller, inverter drive, starter, etc).</t>
       </text>
     </comment>
     <comment ref="K3" authorId="0" shapeId="0">
       <text>
-        <t>Pressure difference across the evaporator</t>
-      </text>
-    </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
-      <text>
-        <t>Pressure difference across the condenser</t>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="0" shapeId="0">
-      <text>
-        <t>Heat transferred to another liquid crossing the control volume boundary from the chiller oil cooler.</t>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="0" shapeId="0">
-      <text>
-        <t>Heat transferred to another liquid crossing the control volume boundary from the chiller auxiliaries (motor, motor controller, inverter drive, starter, etc).</t>
+        <t>The operation state at the operating conditions</t>
       </text>
     </comment>
   </commentList>
@@ -525,6 +532,76 @@
     <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <t>Total power consumed in standby operation</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ASHRAE 205</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <t>Data group defining the grid variables for the evaporator liquid pressure differential</t>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <t>Data group defining the lookup variables for the evaporator liquid pressure differential</t>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <t>Chilled liquid (evaporator) flow</t>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <t>Leaving evaporator liquid temperature</t>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <t>Pressure difference across the evaporator</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ASHRAE 205</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <t>Data group defining the grid variables for the condenser liquid pressure differential</t>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <t>Data group defining the lookup variables for the condenser liquid pressure differential</t>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <t>Condenser liquid flow</t>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <t>Entering condenser liquid temperature</t>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <t>Pressure difference across the condenser</t>
       </text>
     </comment>
   </commentList>
@@ -820,7 +897,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ32"/>
+  <dimension ref="A1:AZ36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,7 +1106,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>1.0.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="D6" s="4" t="n"/>
@@ -1048,7 +1125,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>ASHRAE 90.1-2019 Addendum 'bd' curve set 'AA': 225.0 ton, 2.23 COP liquid-cooled, centrifugal compressor chiller</t>
+          <t>ASHRAE 90.1-2019 Addendum 'bd' curve set 'AA': 150.0-300.0 ton, 5.55 COP, 5.90 IPLV liquid-cooled, centrifugal compressor chiller</t>
         </is>
       </c>
       <c r="D7" s="4" t="n"/>
@@ -1067,7 +1144,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>0d92de87-13de-4fa4-a6f5-c092ded36fa1</t>
+          <t>5adc5b62-8a68-4774-8610-7b157625a90b</t>
         </is>
       </c>
       <c r="D8" s="4" t="n"/>
@@ -1086,7 +1163,7 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>2022-12-20T09:13Z</t>
+          <t>2024-02-22T13:52Z</t>
         </is>
       </c>
       <c r="D9" s="4" t="n"/>
@@ -1104,7 +1181,7 @@
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="4" t="n"/>
       <c r="E10" s="6" t="inlineStr">
@@ -1409,34 +1486,36 @@
       <c r="A29" s="4" t="n"/>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>maximum_power</t>
+          <t>cycling_degradation_coefficient</t>
         </is>
       </c>
       <c r="C29" s="5" t="n">
-        <v>369313.4068244991</v>
+        <v>0</v>
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="E29" s="6" t="n"/>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n"/>
-      <c r="B30" s="4" t="inlineStr">
-        <is>
-          <t>cycling_degradation_coefficient</t>
-        </is>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>performance.performance_map_cooling</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="n"/>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>$performance_map_cooling</t>
+        </is>
+      </c>
+      <c r="D30" s="4" t="n"/>
       <c r="E30" s="6" t="inlineStr">
         <is>
           <t>✓</t>
@@ -1446,13 +1525,13 @@
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>performance.performance_map_cooling</t>
+          <t>performance.performance_map_standby</t>
         </is>
       </c>
       <c r="B31" s="4" t="n"/>
       <c r="C31" s="5" t="inlineStr">
         <is>
-          <t>$performance_map_cooling</t>
+          <t>$performance_map_standby</t>
         </is>
       </c>
       <c r="D31" s="4" t="n"/>
@@ -1465,13 +1544,13 @@
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>performance.performance_map_standby</t>
+          <t>performance.performance_map_evaporator_liquid_pressure_differential</t>
         </is>
       </c>
       <c r="B32" s="4" t="n"/>
       <c r="C32" s="5" t="inlineStr">
         <is>
-          <t>$performance_map_standby</t>
+          <t>$performance_map_evaporator_liqu</t>
         </is>
       </c>
       <c r="D32" s="4" t="n"/>
@@ -1481,32 +1560,98 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>performance.performance_map_condenser_liquid_pressure_differential</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="n"/>
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>$performance_map_condenser_liqui</t>
+        </is>
+      </c>
+      <c r="D33" s="4" t="n"/>
+      <c r="E33" s="6" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>performance.scaling</t>
+        </is>
+      </c>
+      <c r="B34" s="4" t="n"/>
+      <c r="C34" s="5" t="n"/>
+      <c r="D34" s="4" t="n"/>
+      <c r="E34" s="6" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="n"/>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    minimum</t>
+        </is>
+      </c>
+      <c r="C35" s="5" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="D35" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="6" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="n"/>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    maximum</t>
+        </is>
+      </c>
+      <c r="C36" s="5" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="D36" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" s="6" t="n"/>
+    </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation sqref="C5" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"RS0001,RS0002,RS0003,RS0004,RS0005,RS0006,RS0007"</formula1>
     </dataValidation>
-    <dataValidation sqref="C17" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C17" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation sqref="C18" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C18" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"RECIPROCATING,SCREW,CENTRIFUGAL,ROTARY,SCROLL"</formula1>
     </dataValidation>
-    <dataValidation sqref="C22" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C22" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"BY_VOLUME,BY_MASS"</formula1>
     </dataValidation>
-    <dataValidation sqref="C25" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C25" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"BY_VOLUME,BY_MASS"</formula1>
     </dataValidation>
-    <dataValidation sqref="C28" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="C28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"DISCRETE,CONTINUOUS"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C21" r:id="rId1"/>
     <hyperlink ref="C24" r:id="rId2"/>
-    <hyperlink ref="C31" r:id="rId3"/>
-    <hyperlink ref="C32" r:id="rId4"/>
+    <hyperlink ref="C30" r:id="rId3"/>
+    <hyperlink ref="C31" r:id="rId4"/>
+    <hyperlink ref="C32" r:id="rId5"/>
+    <hyperlink ref="C33" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="anysvml"/>
@@ -1667,7 +1812,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="A4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"WATER,PROPYLENE_GLYCOL,ETHYLENE_GLYCOL,SODIUM_CHLORIDE,CALCIUM_CHLORIDE,ETHANOL,METHANOL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1830,7 +1975,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="A4" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="A4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"WATER,PROPYLENE_GLYCOL,ETHYLENE_GLYCOL,SODIUM_CHLORIDE,CALCIUM_CHLORIDE,ETHANOL,METHANOL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1985,9 +2130,6 @@
       <c r="I2" s="4" t="n"/>
       <c r="J2" s="4" t="n"/>
       <c r="K2" s="4" t="n"/>
-      <c r="L2" s="4" t="n"/>
-      <c r="M2" s="4" t="n"/>
-      <c r="N2" s="4" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="8" t="inlineStr">
@@ -2032,32 +2174,17 @@
       </c>
       <c r="I3" s="9" t="inlineStr">
         <is>
-          <t>evaporator_liquid_entering_temperature</t>
+          <t>oil_cooler_heat</t>
         </is>
       </c>
       <c r="J3" s="9" t="inlineStr">
         <is>
-          <t>condenser_liquid_leaving_temperature</t>
+          <t>auxiliary_heat</t>
         </is>
       </c>
       <c r="K3" s="9" t="inlineStr">
         <is>
-          <t>evaporator_liquid_differential_pressure</t>
-        </is>
-      </c>
-      <c r="L3" s="9" t="inlineStr">
-        <is>
-          <t>condenser_liquid_differential_pressure</t>
-        </is>
-      </c>
-      <c r="M3" s="9" t="inlineStr">
-        <is>
-          <t>oil_cooler_heat</t>
-        </is>
-      </c>
-      <c r="N3" s="9" t="inlineStr">
-        <is>
-          <t>auxiliary_heat</t>
+          <t>operation_state</t>
         </is>
       </c>
     </row>
@@ -2104,32 +2231,17 @@
       </c>
       <c r="I4" s="4" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>W</t>
         </is>
       </c>
       <c r="J4" s="4" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>W</t>
         </is>
       </c>
       <c r="K4" s="4" t="inlineStr">
         <is>
-          <t>Pa</t>
-        </is>
-      </c>
-      <c r="L4" s="4" t="inlineStr">
-        <is>
-          <t>Pa</t>
-        </is>
-      </c>
-      <c r="M4" s="4" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="N4" s="4" t="inlineStr">
-        <is>
-          <t>W</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2253,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2150,31 +2262,24 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>107768.9247186337</v>
+        <v>43277.37423929632</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>198295.1326754816</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>306064.0573941154</v>
+        <v>241572.5069147779</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>278.4288747660367</v>
+        <v>0</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>287.2986041267702</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L5" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -2185,7 +2290,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2194,31 +2299,24 @@
         <v>2</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>142848.3336671182</v>
+        <v>57364.41011833567</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>396590.2653509632</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>539438.5990180814</v>
+        <v>453954.6754692989</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>279.8188606431845</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>288.3438623435173</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -2229,7 +2327,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2238,31 +2336,24 @@
         <v>3</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>199053.1147857721</v>
+        <v>79934.88071419891</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>594885.3980264448</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>793938.512812217</v>
+        <v>674820.2787406438</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>281.2088465203323</v>
+        <v>0</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>289.4837387165082</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -2273,7 +2364,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2282,31 +2373,24 @@
         <v>4</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>276383.2680745955</v>
+        <v>110988.7860268861</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>793180.5307019264</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>1069563.798776522</v>
+        <v>904169.3167288125</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>282.59883239748</v>
+        <v>0</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>290.718233245743</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L8" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -2317,7 +2401,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>295.0018518518519</v>
@@ -2326,31 +2410,24 @@
         <v>1</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>128340.5287076803</v>
+        <v>51538.42914785137</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>189751.5752031771</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>318092.1039108573</v>
+        <v>241290.0043510284</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>278.3689871426398</v>
+        <v>0</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>296.4316476774228</v>
-      </c>
-      <c r="K9" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L9" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K9" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -2361,7 +2438,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>295.0018518518519</v>
@@ -2370,31 +2447,24 @@
         <v>2</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>170116.1138585544</v>
+        <v>68314.48622887158</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>379503.1504063542</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>549619.2642649085</v>
+        <v>447817.6366352257</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>279.6990853963907</v>
+        <v>0</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>297.4723417509647</v>
-      </c>
-      <c r="K10" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L10" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -2405,7 +2475,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>295.0018518518519</v>
@@ -2414,31 +2484,24 @@
         <v>3</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>237049.6138772315</v>
+        <v>95193.34891602416</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>569254.7256095313</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>806304.3394867628</v>
+        <v>664448.0745255555</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>281.0291836501416</v>
+        <v>0</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>298.626118422961</v>
-      </c>
-      <c r="K11" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L11" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M11" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K11" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -2449,7 +2512,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>295.0018518518519</v>
@@ -2458,31 +2521,24 @@
         <v>4</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>329141.0287637117</v>
+        <v>132175.0172093091</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>759006.3008127083</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>1088147.32957642</v>
+        <v>891181.3180220174</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>282.3592819038925</v>
+        <v>0</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>299.8929776934116</v>
-      </c>
-      <c r="K12" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L12" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K12" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -2493,7 +2549,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>304.075925925926</v>
@@ -2502,31 +2558,24 @@
         <v>1</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>130462.0143640797</v>
+        <v>52390.3660947496</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>176060.8477971277</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>306522.8621612074</v>
+        <v>228451.2138918773</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>278.2730194933812</v>
+        <v>0</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>305.4581605799536</v>
-      </c>
-      <c r="K13" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L13" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M13" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K13" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -2537,7 +2586,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>304.075925925926</v>
@@ -2546,31 +2595,24 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>172928.155378933</v>
+        <v>69443.73358446687</v>
       </c>
       <c r="G14" s="5" t="n">
         <v>352121.6955942554</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>525049.8509731884</v>
+        <v>421565.4291787223</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>279.5071500978735</v>
+        <v>0</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>306.4435865108174</v>
-      </c>
-      <c r="K14" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L14" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K14" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -2581,7 +2623,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>304.075925925926</v>
@@ -2590,31 +2632,24 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>240968.074871272</v>
+        <v>96766.90737291625</v>
       </c>
       <c r="G15" s="5" t="n">
         <v>528182.5433913831</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>769150.6182626551</v>
+        <v>624949.4507642994</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>280.7412807023658</v>
+        <v>0</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>307.544334876676</v>
-      </c>
-      <c r="K15" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L15" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K15" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -2625,7 +2660,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>304.075925925926</v>
@@ -2634,31 +2669,24 @@
         <v>4</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>334581.7728410967</v>
+        <v>134359.8874600978</v>
       </c>
       <c r="G16" s="5" t="n">
         <v>704243.3911885108</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>1038825.164029608</v>
+        <v>838603.2786486086</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>281.9754113068581</v>
+        <v>0</v>
       </c>
       <c r="J16" s="5" t="n">
-        <v>308.7604056775293</v>
-      </c>
-      <c r="K16" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L16" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K16" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -2669,7 +2697,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>313.15</v>
@@ -2678,31 +2706,24 @@
         <v>1</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>115937.8962271962</v>
+        <v>46557.8341496946</v>
       </c>
       <c r="G17" s="5" t="n">
         <v>157222.9504573334</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>273160.8466845297</v>
+        <v>203780.784607028</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>278.1409718182609</v>
+        <v>0</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>314.3857724962206</v>
-      </c>
-      <c r="K17" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L17" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M17" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K17" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -2713,7 +2734,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>313.15</v>
@@ -2722,31 +2743,24 @@
         <v>2</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>153676.3526978263</v>
+        <v>61712.67872253335</v>
       </c>
       <c r="G18" s="5" t="n">
         <v>314445.9009146669</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>468122.2536124932</v>
+        <v>376158.5796372002</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>279.2430547476328</v>
+        <v>0</v>
       </c>
       <c r="J18" s="5" t="n">
-        <v>315.2677727807794</v>
-      </c>
-      <c r="K18" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L18" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M18" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -2757,7 +2771,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>313.15</v>
@@ -2766,31 +2780,24 @@
         <v>3</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>214141.5016061932</v>
+        <v>85994.00921343433</v>
       </c>
       <c r="G19" s="5" t="n">
         <v>471668.8513720003</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>685810.3529781936</v>
+        <v>557662.8605854346</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>280.3451376770048</v>
+        <v>0</v>
       </c>
       <c r="J19" s="5" t="n">
-        <v>316.2525880250422</v>
-      </c>
-      <c r="K19" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L19" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M19" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -2801,7 +2808,7 @@
         <v>277.0388888888889</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>313.15</v>
@@ -2810,31 +2817,24 @@
         <v>4</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>297333.3429522971</v>
+        <v>119401.8256223976</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>628891.8018293338</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>926225.1447816308</v>
+        <v>748293.6274517314</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>281.4472206063768</v>
+        <v>0</v>
       </c>
       <c r="J20" s="5" t="n">
-        <v>317.3402182290092</v>
-      </c>
-      <c r="K20" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L20" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M20" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K20" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -2845,7 +2845,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C21" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2854,31 +2854,24 @@
         <v>1</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>104139.1616403997</v>
+        <v>41819.74983089806</v>
       </c>
       <c r="G21" s="5" t="n">
         <v>215062.2804504816</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>319201.4420908813</v>
+        <v>256882.0302813796</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>282.4385859979556</v>
+        <v>0</v>
       </c>
       <c r="J21" s="5" t="n">
-        <v>287.3574449892109</v>
-      </c>
-      <c r="K21" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L21" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M21" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K21" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -2889,7 +2882,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2898,31 +2891,24 @@
         <v>2</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>138037.0616915845</v>
+        <v>55432.32052575751</v>
       </c>
       <c r="G22" s="5" t="n">
         <v>430124.5609009632</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>568161.6225925477</v>
+        <v>485556.8814267207</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>283.9493942181334</v>
+        <v>0</v>
       </c>
       <c r="J22" s="5" t="n">
-        <v>288.4725095223917</v>
-      </c>
-      <c r="K22" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L22" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M22" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K22" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -2933,7 +2919,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2942,31 +2928,24 @@
         <v>3</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>192348.8106596686</v>
+        <v>77242.59553610178</v>
       </c>
       <c r="G23" s="5" t="n">
         <v>645186.8413514448</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>837535.6520111134</v>
+        <v>722429.4368875467</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>285.4602024383111</v>
+        <v>0</v>
       </c>
       <c r="J23" s="5" t="n">
-        <v>289.6790053795179</v>
-      </c>
-      <c r="K23" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L23" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M23" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K23" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -2977,7 +2956,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>285.9277777777778</v>
@@ -2986,31 +2965,24 @@
         <v>4</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>267074.4085446518</v>
+        <v>107250.5748619308</v>
       </c>
       <c r="G24" s="5" t="n">
         <v>860249.1218019264</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>1127323.530346578</v>
+        <v>967499.6966638572</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>286.9710106584889</v>
+        <v>0</v>
       </c>
       <c r="J24" s="5" t="n">
-        <v>290.9769325605894</v>
-      </c>
-      <c r="K24" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L24" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M24" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K24" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -3021,7 +2993,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3030,31 +3002,24 @@
         <v>1</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>131680.5311535259</v>
+        <v>52879.69274667089</v>
       </c>
       <c r="G25" s="5" t="n">
         <v>211042.2755781771</v>
       </c>
       <c r="H25" s="5" t="n">
-        <v>342722.806731703</v>
+        <v>263921.968324848</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>282.4103455441042</v>
+        <v>0</v>
       </c>
       <c r="J25" s="5" t="n">
-        <v>296.5423605044347</v>
-      </c>
-      <c r="K25" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L25" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M25" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K25" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -3065,7 +3030,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3074,31 +3039,24 @@
         <v>2</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>174543.3064382225</v>
+        <v>70092.3388946559</v>
       </c>
       <c r="G26" s="5" t="n">
         <v>422084.5511563543</v>
       </c>
       <c r="H26" s="5" t="n">
-        <v>596627.8575945768</v>
+        <v>492176.8900510102</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>283.8929133104306</v>
+        <v>0</v>
       </c>
       <c r="J26" s="5" t="n">
-        <v>297.6836412132348</v>
-      </c>
-      <c r="K26" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L26" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K26" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -3109,7 +3067,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3118,31 +3076,24 @@
         <v>3</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>243218.7196001795</v>
+        <v>97670.71145620767</v>
       </c>
       <c r="G27" s="5" t="n">
         <v>633126.8267345314</v>
       </c>
       <c r="H27" s="5" t="n">
-        <v>876345.5463347109</v>
+        <v>730797.5381907391</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>285.375481076757</v>
+        <v>0</v>
       </c>
       <c r="J27" s="5" t="n">
-        <v>298.9409474424113</v>
-      </c>
-      <c r="K27" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L27" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M27" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -3153,7 +3104,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C28" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D28" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3162,31 +3113,24 @@
         <v>4</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>337706.7706393968</v>
+        <v>135614.8104313262</v>
       </c>
       <c r="G28" s="5" t="n">
         <v>844169.1023127085</v>
       </c>
       <c r="H28" s="5" t="n">
-        <v>1181875.872952105</v>
+        <v>979783.9127440348</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>286.8580488430835</v>
+        <v>0</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>300.3142791919643</v>
-      </c>
-      <c r="K28" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L28" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M28" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K28" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -3197,7 +3141,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C29" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>304.075925925926</v>
@@ -3206,31 +3150,24 @@
         <v>1</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>140391.9783673006</v>
+        <v>56377.99768216794</v>
       </c>
       <c r="G29" s="5" t="n">
         <v>201875.1007721278</v>
       </c>
       <c r="H29" s="5" t="n">
-        <v>342267.0791394284</v>
+        <v>258253.0984542957</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>282.3459463243815</v>
+        <v>0</v>
       </c>
       <c r="J29" s="5" t="n">
-        <v>305.6193456055665</v>
-      </c>
-      <c r="K29" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L29" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M29" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K29" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -3241,7 +3178,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C30" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>304.075925925926</v>
@@ -3250,31 +3187,24 @@
         <v>2</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>186090.3801569753</v>
+        <v>74729.36234088505</v>
       </c>
       <c r="G30" s="5" t="n">
         <v>403750.2015442555</v>
       </c>
       <c r="H30" s="5" t="n">
-        <v>589840.5817012308</v>
+        <v>478479.5638851406</v>
       </c>
       <c r="I30" s="5" t="n">
-        <v>283.7641148709853</v>
+        <v>0</v>
       </c>
       <c r="J30" s="5" t="n">
-        <v>306.7357539290668</v>
-      </c>
-      <c r="K30" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L30" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M30" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K30" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -3285,7 +3215,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C31" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>304.075925925926</v>
@@ -3294,31 +3224,24 @@
         <v>3</v>
       </c>
       <c r="F31" s="5" t="n">
-        <v>259309.0787340484</v>
+        <v>104132.2076221866</v>
       </c>
       <c r="G31" s="5" t="n">
         <v>605625.3023163833</v>
       </c>
       <c r="H31" s="5" t="n">
-        <v>864934.3810504318</v>
+        <v>709757.50993857</v>
       </c>
       <c r="I31" s="5" t="n">
-        <v>285.1822834175891</v>
+        <v>0</v>
       </c>
       <c r="J31" s="5" t="n">
-        <v>307.9762623201461</v>
-      </c>
-      <c r="K31" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L31" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M31" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K31" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -3329,7 +3252,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C32" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D32" s="5" t="n">
         <v>304.075925925926</v>
@@ -3338,31 +3261,24 @@
         <v>4</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>360048.07409852</v>
+        <v>144586.5335260727</v>
       </c>
       <c r="G32" s="5" t="n">
         <v>807500.4030885111</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>1167548.477187031</v>
+        <v>952086.9366145838</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>286.6004519641928</v>
+        <v>0</v>
       </c>
       <c r="J32" s="5" t="n">
-        <v>309.3408707788041</v>
-      </c>
-      <c r="K32" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L32" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M32" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K32" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -3373,7 +3289,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>313.15</v>
@@ -3382,31 +3298,24 @@
         <v>1</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>131046.3194767919</v>
+        <v>52625.0087906733</v>
       </c>
       <c r="G33" s="5" t="n">
         <v>187560.7560323336</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>318607.0755091255</v>
+        <v>240185.7648230069</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>282.2453883387876</v>
+        <v>0</v>
       </c>
       <c r="J33" s="5" t="n">
-        <v>314.5913700418427</v>
-      </c>
-      <c r="K33" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L33" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M33" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K33" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -3417,7 +3326,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C34" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D34" s="5" t="n">
         <v>313.15</v>
@@ -3426,31 +3335,24 @@
         <v>2</v>
       </c>
       <c r="F34" s="5" t="n">
-        <v>173702.6551887996</v>
+        <v>69754.75383643071</v>
       </c>
       <c r="G34" s="5" t="n">
         <v>375121.5120646671</v>
       </c>
       <c r="H34" s="5" t="n">
-        <v>548824.1672534668</v>
+        <v>444876.2659010979</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>283.5629988997974</v>
+        <v>0</v>
       </c>
       <c r="J34" s="5" t="n">
-        <v>315.6328661185704</v>
-      </c>
-      <c r="K34" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L34" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M34" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K34" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -3461,7 +3363,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C35" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D35" s="5" t="n">
         <v>313.15</v>
@@ -3470,31 +3372,24 @@
         <v>3</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>242047.307618321</v>
+        <v>97200.3009472447</v>
       </c>
       <c r="G35" s="5" t="n">
         <v>562682.2680970007</v>
       </c>
       <c r="H35" s="5" t="n">
-        <v>804729.5757153217</v>
+        <v>659882.5690442454</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>284.8806094608072</v>
+        <v>0</v>
       </c>
       <c r="J35" s="5" t="n">
-        <v>316.7905754654611</v>
-      </c>
-      <c r="K35" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L35" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M35" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K35" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -3505,7 +3400,7 @@
         <v>280.9277777777778</v>
       </c>
       <c r="C36" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>313.15</v>
@@ -3514,31 +3409,24 @@
         <v>4</v>
       </c>
       <c r="F36" s="5" t="n">
-        <v>336080.2767653561</v>
+        <v>134961.6501231153</v>
       </c>
       <c r="G36" s="5" t="n">
         <v>750243.0241293343</v>
       </c>
       <c r="H36" s="5" t="n">
-        <v>1086323.30089469</v>
+        <v>885204.6742524495</v>
       </c>
       <c r="I36" s="5" t="n">
-        <v>286.1982200218171</v>
+        <v>0</v>
       </c>
       <c r="J36" s="5" t="n">
-        <v>318.0644980825148</v>
-      </c>
-      <c r="K36" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L36" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M36" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K36" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -3549,7 +3437,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C37" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>285.9277777777778</v>
@@ -3558,31 +3446,24 @@
         <v>1</v>
       </c>
       <c r="F37" s="5" t="n">
-        <v>97153.09668534776</v>
+        <v>39014.3163693583</v>
       </c>
       <c r="G37" s="5" t="n">
         <v>220574.3985421481</v>
       </c>
       <c r="H37" s="5" t="n">
-        <v>317727.4952274959</v>
+        <v>259588.7149115065</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>286.3690940473181</v>
+        <v>0</v>
       </c>
       <c r="J37" s="5" t="n">
-        <v>287.3508433476639</v>
-      </c>
-      <c r="K37" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L37" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M37" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K37" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -3593,7 +3474,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C38" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>285.9277777777778</v>
@@ -3602,31 +3483,24 @@
         <v>2</v>
       </c>
       <c r="F38" s="5" t="n">
-        <v>128776.9921462597</v>
+        <v>51713.70222979488</v>
       </c>
       <c r="G38" s="5" t="n">
         <v>441148.7970842963</v>
       </c>
       <c r="H38" s="5" t="n">
-        <v>569925.789230556</v>
+        <v>492862.4993140912</v>
       </c>
       <c r="I38" s="5" t="n">
-        <v>287.9215214279695</v>
+        <v>0</v>
       </c>
       <c r="J38" s="5" t="n">
-        <v>288.4804110255345</v>
-      </c>
-      <c r="K38" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L38" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M38" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K38" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -3637,7 +3511,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C39" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D39" s="5" t="n">
         <v>285.9277777777778</v>
@@ -3646,31 +3520,24 @@
         <v>3</v>
       </c>
       <c r="F39" s="5" t="n">
-        <v>179445.2951701207</v>
+        <v>72060.85812616021</v>
       </c>
       <c r="G39" s="5" t="n">
         <v>661723.1956264444</v>
       </c>
       <c r="H39" s="5" t="n">
-        <v>841168.4907965651</v>
+        <v>733784.0537526046</v>
       </c>
       <c r="I39" s="5" t="n">
-        <v>289.473948808621</v>
+        <v>0</v>
       </c>
       <c r="J39" s="5" t="n">
-        <v>289.6952764541783</v>
-      </c>
-      <c r="K39" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L39" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M39" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K39" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -3681,7 +3548,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C40" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>285.9277777777778</v>
@@ -3690,31 +3557,24 @@
         <v>4</v>
       </c>
       <c r="F40" s="5" t="n">
-        <v>249158.0057569306</v>
+        <v>100055.7840584543</v>
       </c>
       <c r="G40" s="5" t="n">
         <v>882297.5941685926</v>
       </c>
       <c r="H40" s="5" t="n">
-        <v>1131455.599925523</v>
+        <v>982353.3782270469</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>291.0263761892725</v>
+        <v>0</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>290.9954396335953</v>
-      </c>
-      <c r="K40" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L40" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M40" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K40" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -3725,7 +3585,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C41" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3734,31 +3594,24 @@
         <v>1</v>
       </c>
       <c r="F41" s="5" t="n">
-        <v>129777.7102712454</v>
+        <v>52115.56624501193</v>
       </c>
       <c r="G41" s="5" t="n">
         <v>221077.9462698436</v>
       </c>
       <c r="H41" s="5" t="n">
-        <v>350855.6565410891</v>
+        <v>273193.5125148556</v>
       </c>
       <c r="I41" s="5" t="n">
-        <v>286.3726380727585</v>
+        <v>0</v>
       </c>
       <c r="J41" s="5" t="n">
-        <v>296.5789169437945</v>
-      </c>
-      <c r="K41" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L41" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M41" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K41" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -3769,7 +3622,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C42" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D42" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3778,31 +3631,24 @@
         <v>2</v>
       </c>
       <c r="F42" s="5" t="n">
-        <v>172021.1063419478</v>
+        <v>69079.4847926237</v>
       </c>
       <c r="G42" s="5" t="n">
         <v>442155.8925396873</v>
       </c>
       <c r="H42" s="5" t="n">
-        <v>614176.9988816351</v>
+        <v>511235.377332311</v>
       </c>
       <c r="I42" s="5" t="n">
-        <v>287.9286094788504</v>
+        <v>0</v>
       </c>
       <c r="J42" s="5" t="n">
-        <v>297.7625230485463</v>
-      </c>
-      <c r="K42" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L42" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M42" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K42" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -3813,7 +3659,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C43" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D43" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3822,31 +3668,24 @@
         <v>3</v>
       </c>
       <c r="F43" s="5" t="n">
-        <v>239704.1403790709</v>
+        <v>96259.34207822896</v>
       </c>
       <c r="G43" s="5" t="n">
         <v>663233.8388095309</v>
       </c>
       <c r="H43" s="5" t="n">
-        <v>902937.9791886018</v>
+        <v>759493.1808877599</v>
       </c>
       <c r="I43" s="5" t="n">
-        <v>289.4845808849423</v>
+        <v>0</v>
       </c>
       <c r="J43" s="5" t="n">
-        <v>299.0604780721214</v>
-      </c>
-      <c r="K43" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L43" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M43" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K43" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -3857,7 +3696,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C44" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>295.0018518518519</v>
@@ -3866,31 +3705,24 @@
         <v>4</v>
       </c>
       <c r="F44" s="5" t="n">
-        <v>332826.8123826145</v>
+        <v>133655.1381018278</v>
       </c>
       <c r="G44" s="5" t="n">
         <v>884311.7850793746</v>
       </c>
       <c r="H44" s="5" t="n">
-        <v>1217138.597461989</v>
+        <v>1017966.923181202</v>
       </c>
       <c r="I44" s="5" t="n">
-        <v>291.0405522910341</v>
+        <v>0</v>
       </c>
       <c r="J44" s="5" t="n">
-        <v>300.4727820145197</v>
-      </c>
-      <c r="K44" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L44" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M44" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N44" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K44" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -3901,7 +3733,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C45" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D45" s="5" t="n">
         <v>304.075925925926</v>
@@ -3910,31 +3742,24 @@
         <v>1</v>
       </c>
       <c r="F45" s="5" t="n">
-        <v>144004.7692283221</v>
+        <v>57828.8064616834</v>
       </c>
       <c r="G45" s="5" t="n">
         <v>216434.3240637943</v>
       </c>
       <c r="H45" s="5" t="n">
-        <v>360439.0932921164</v>
+        <v>274263.1305254777</v>
       </c>
       <c r="I45" s="5" t="n">
-        <v>286.3399557383366</v>
+        <v>0</v>
       </c>
       <c r="J45" s="5" t="n">
-        <v>305.7012905134217</v>
-      </c>
-      <c r="K45" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L45" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M45" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N45" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K45" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -3945,7 +3770,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C46" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D46" s="5" t="n">
         <v>304.075925925926</v>
@@ -3954,31 +3779,24 @@
         <v>2</v>
       </c>
       <c r="F46" s="5" t="n">
-        <v>190879.1553603292</v>
+        <v>76652.41777791841</v>
       </c>
       <c r="G46" s="5" t="n">
         <v>432868.6481275886</v>
       </c>
       <c r="H46" s="5" t="n">
-        <v>623747.8034879178</v>
+        <v>509521.065905507</v>
       </c>
       <c r="I46" s="5" t="n">
-        <v>287.8632448100065</v>
+        <v>0</v>
       </c>
       <c r="J46" s="5" t="n">
-        <v>306.8886552058098</v>
-      </c>
-      <c r="K46" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L46" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M46" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N46" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K46" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -3989,7 +3807,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C47" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D47" s="5" t="n">
         <v>304.075925925926</v>
@@ -3998,31 +3816,24 @@
         <v>3</v>
       </c>
       <c r="F47" s="5" t="n">
-        <v>265982.0345590549</v>
+        <v>106811.9040864046</v>
       </c>
       <c r="G47" s="5" t="n">
         <v>649302.9721913829</v>
       </c>
       <c r="H47" s="5" t="n">
-        <v>915285.0067504378</v>
+        <v>756114.8762777875</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>289.3865338816765</v>
+        <v>0</v>
       </c>
       <c r="J47" s="5" t="n">
-        <v>308.2033135071401</v>
-      </c>
-      <c r="K47" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L47" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M47" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N47" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K47" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -4033,7 +3844,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C48" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D48" s="5" t="n">
         <v>304.075925925926</v>
@@ -4042,31 +3853,24 @@
         <v>4</v>
       </c>
       <c r="F48" s="5" t="n">
-        <v>369313.4068244991</v>
+        <v>148307.265387142</v>
       </c>
       <c r="G48" s="5" t="n">
         <v>865737.2962551771</v>
       </c>
       <c r="H48" s="5" t="n">
-        <v>1235050.703079676</v>
+        <v>1014044.561642319</v>
       </c>
       <c r="I48" s="5" t="n">
-        <v>290.9098229533464</v>
+        <v>0</v>
       </c>
       <c r="J48" s="5" t="n">
-        <v>309.6452654174127</v>
-      </c>
-      <c r="K48" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L48" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M48" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K48" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -4077,7 +3881,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C49" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D49" s="5" t="n">
         <v>313.15</v>
@@ -4086,31 +3890,24 @@
         <v>1</v>
       </c>
       <c r="F49" s="5" t="n">
-        <v>139575.3914073492</v>
+        <v>56050.07625623728</v>
       </c>
       <c r="G49" s="5" t="n">
         <v>206643.531924</v>
       </c>
       <c r="H49" s="5" t="n">
-        <v>346218.9233313492</v>
+        <v>262693.6081802373</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>286.2710470440523</v>
+        <v>0</v>
       </c>
       <c r="J49" s="5" t="n">
-        <v>314.7162853162046</v>
-      </c>
-      <c r="K49" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L49" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M49" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N49" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K49" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -4121,7 +3918,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C50" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D50" s="5" t="n">
         <v>313.15</v>
@@ -4130,31 +3927,24 @@
         <v>2</v>
       </c>
       <c r="F50" s="5" t="n">
-        <v>185007.9894137448</v>
+        <v>74294.70059223869</v>
       </c>
       <c r="G50" s="5" t="n">
         <v>413287.063848</v>
       </c>
       <c r="H50" s="5" t="n">
-        <v>598295.0532617448</v>
+        <v>487581.7644402387</v>
       </c>
       <c r="I50" s="5" t="n">
-        <v>287.7254274214379</v>
+        <v>0</v>
       </c>
       <c r="J50" s="5" t="n">
-        <v>315.8566711075895</v>
-      </c>
-      <c r="K50" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L50" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M50" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N50" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K50" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -4165,7 +3955,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C51" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>313.15</v>
@@ -4174,31 +3964,24 @@
         <v>3</v>
       </c>
       <c r="F51" s="5" t="n">
-        <v>257800.812985864</v>
+        <v>103526.5248485401</v>
       </c>
       <c r="G51" s="5" t="n">
         <v>619930.595772</v>
       </c>
       <c r="H51" s="5" t="n">
-        <v>877731.408757864</v>
+        <v>723457.1206205401</v>
       </c>
       <c r="I51" s="5" t="n">
-        <v>289.1798077988236</v>
+        <v>0</v>
       </c>
       <c r="J51" s="5" t="n">
-        <v>317.1208338408565</v>
-      </c>
-      <c r="K51" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L51" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M51" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K51" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -4209,7 +3992,7 @@
         <v>284.8166666666667</v>
       </c>
       <c r="C52" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>313.15</v>
@@ -4218,31 +4001,24 @@
         <v>4</v>
       </c>
       <c r="F52" s="5" t="n">
-        <v>357953.8621237071</v>
+        <v>143745.5490251415</v>
       </c>
       <c r="G52" s="5" t="n">
         <v>826574.127696</v>
       </c>
       <c r="H52" s="5" t="n">
-        <v>1184527.989819707</v>
+        <v>970319.6767211416</v>
       </c>
       <c r="I52" s="5" t="n">
-        <v>290.6341881762092</v>
+        <v>0</v>
       </c>
       <c r="J52" s="5" t="n">
-        <v>318.5087735160055</v>
-      </c>
-      <c r="K52" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L52" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M52" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K52" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -4253,7 +4029,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C53" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>285.9277777777778</v>
@@ -4262,31 +4038,24 @@
         <v>1</v>
       </c>
       <c r="F53" s="5" t="n">
-        <v>88544.65241093158</v>
+        <v>35557.37490450928</v>
       </c>
       <c r="G53" s="5" t="n">
         <v>214831.4869504814</v>
       </c>
       <c r="H53" s="5" t="n">
-        <v>303376.139361413</v>
+        <v>250388.8618549907</v>
       </c>
       <c r="I53" s="5" t="n">
-        <v>290.220068515395</v>
+        <v>0</v>
       </c>
       <c r="J53" s="5" t="n">
-        <v>287.2865652454506</v>
-      </c>
-      <c r="K53" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L53" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M53" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K53" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -4297,7 +4066,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C54" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>285.9277777777778</v>
@@ -4306,31 +4075,24 @@
         <v>2</v>
       </c>
       <c r="F54" s="5" t="n">
-        <v>117366.4494199856</v>
+        <v>47131.50630339288</v>
       </c>
       <c r="G54" s="5" t="n">
         <v>429662.9739009627</v>
       </c>
       <c r="H54" s="5" t="n">
-        <v>547029.4233209483</v>
+        <v>476794.4802043556</v>
       </c>
       <c r="I54" s="5" t="n">
-        <v>291.7345814752344</v>
+        <v>0</v>
       </c>
       <c r="J54" s="5" t="n">
-        <v>288.3778607883315</v>
-      </c>
-      <c r="K54" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L54" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M54" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K54" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -4341,7 +4103,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C55" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>285.9277777777778</v>
@@ -4350,31 +4112,24 @@
         <v>3</v>
       </c>
       <c r="F55" s="5" t="n">
-        <v>163545.1862031245</v>
+        <v>65675.76179150869</v>
       </c>
       <c r="G55" s="5" t="n">
         <v>644494.4608514442</v>
       </c>
       <c r="H55" s="5" t="n">
-        <v>808039.6470545686</v>
+        <v>710170.2226429528</v>
       </c>
       <c r="I55" s="5" t="n">
-        <v>293.2490944350739</v>
+        <v>0</v>
       </c>
       <c r="J55" s="5" t="n">
-        <v>289.5468961043265</v>
-      </c>
-      <c r="K55" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L55" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M55" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K55" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -4385,7 +4140,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C56" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D56" s="5" t="n">
         <v>285.9277777777778</v>
@@ -4394,31 +4149,24 @@
         <v>4</v>
       </c>
       <c r="F56" s="5" t="n">
-        <v>227080.8627603484</v>
+        <v>91190.1413688567</v>
       </c>
       <c r="G56" s="5" t="n">
         <v>859325.9478019255</v>
       </c>
       <c r="H56" s="5" t="n">
-        <v>1086406.810562274</v>
+        <v>950516.0891707821</v>
       </c>
       <c r="I56" s="5" t="n">
-        <v>294.7636073949133</v>
+        <v>0</v>
       </c>
       <c r="J56" s="5" t="n">
-        <v>290.7936711934357</v>
-      </c>
-      <c r="K56" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L56" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M56" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K56" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -4429,7 +4177,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C57" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D57" s="5" t="n">
         <v>295.0018518518519</v>
@@ -4438,31 +4186,24 @@
         <v>1</v>
       </c>
       <c r="F57" s="5" t="n">
-        <v>124344.9946881798</v>
+        <v>49933.92004191739</v>
       </c>
       <c r="G57" s="5" t="n">
         <v>219858.5872781769</v>
       </c>
       <c r="H57" s="5" t="n">
-        <v>344203.5819663567</v>
+        <v>269792.5073200943</v>
       </c>
       <c r="I57" s="5" t="n">
-        <v>290.2555084255533</v>
+        <v>0</v>
       </c>
       <c r="J57" s="5" t="n">
-        <v>296.5490164579245</v>
-      </c>
-      <c r="K57" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L57" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M57" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N57" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K57" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -4473,7 +4214,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C58" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D58" s="5" t="n">
         <v>295.0018518518519</v>
@@ -4482,31 +4223,24 @@
         <v>2</v>
       </c>
       <c r="F58" s="5" t="n">
-        <v>164820.0103826585</v>
+        <v>66187.70011928766</v>
       </c>
       <c r="G58" s="5" t="n">
         <v>439717.1745563538</v>
       </c>
       <c r="H58" s="5" t="n">
-        <v>604537.1849390122</v>
+        <v>505904.8746756414</v>
       </c>
       <c r="I58" s="5" t="n">
-        <v>291.8054612955511</v>
+        <v>0</v>
       </c>
       <c r="J58" s="5" t="n">
-        <v>297.7191929389177</v>
-      </c>
-      <c r="K58" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L58" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M58" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K58" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -4517,7 +4251,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C59" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D59" s="5" t="n">
         <v>295.0018518518519</v>
@@ -4526,31 +4260,24 @@
         <v>3</v>
       </c>
       <c r="F59" s="5" t="n">
-        <v>229669.7175491338</v>
+        <v>92229.7623712744</v>
       </c>
       <c r="G59" s="5" t="n">
         <v>659575.7618345306</v>
       </c>
       <c r="H59" s="5" t="n">
-        <v>889245.4793836644</v>
+        <v>751805.524205805</v>
       </c>
       <c r="I59" s="5" t="n">
-        <v>293.3554141655488</v>
+        <v>0</v>
       </c>
       <c r="J59" s="5" t="n">
-        <v>298.9989314985912</v>
-      </c>
-      <c r="K59" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L59" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M59" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N59" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K59" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -4561,7 +4288,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C60" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D60" s="5" t="n">
         <v>295.0018518518519</v>
@@ -4570,31 +4297,24 @@
         <v>4</v>
       </c>
       <c r="F60" s="5" t="n">
-        <v>318894.116187606</v>
+        <v>128060.1067978776</v>
       </c>
       <c r="G60" s="5" t="n">
         <v>879434.3491127075</v>
       </c>
       <c r="H60" s="5" t="n">
-        <v>1198328.465300314</v>
+        <v>1007494.455910585</v>
       </c>
       <c r="I60" s="5" t="n">
-        <v>294.9053670355466</v>
+        <v>0</v>
       </c>
       <c r="J60" s="5" t="n">
-        <v>300.3882321369449</v>
-      </c>
-      <c r="K60" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L60" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M60" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N60" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K60" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -4605,7 +4325,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C61" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D61" s="5" t="n">
         <v>304.075925925926</v>
@@ -4614,31 +4334,24 @@
         <v>1</v>
       </c>
       <c r="F61" s="5" t="n">
-        <v>142992.321644372</v>
+        <v>57422.23218154954</v>
       </c>
       <c r="G61" s="5" t="n">
         <v>219738.5176721275</v>
       </c>
       <c r="H61" s="5" t="n">
-        <v>362730.8393164995</v>
+        <v>277160.7498536771</v>
       </c>
       <c r="I61" s="5" t="n">
-        <v>290.2546619622298</v>
+        <v>0</v>
       </c>
       <c r="J61" s="5" t="n">
-        <v>305.7116249163788</v>
-      </c>
-      <c r="K61" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L61" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M61" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K61" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -4649,7 +4362,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C62" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D62" s="5" t="n">
         <v>304.075925925926</v>
@@ -4658,31 +4371,24 @@
         <v>2</v>
       </c>
       <c r="F62" s="5" t="n">
-        <v>189537.1502260091</v>
+        <v>76113.50121564722</v>
       </c>
       <c r="G62" s="5" t="n">
         <v>439477.035344255</v>
       </c>
       <c r="H62" s="5" t="n">
-        <v>629014.1855702641</v>
+        <v>515590.5365599022</v>
       </c>
       <c r="I62" s="5" t="n">
-        <v>291.803768368904</v>
+        <v>0</v>
       </c>
       <c r="J62" s="5" t="n">
-        <v>306.9124034370649</v>
-      </c>
-      <c r="K62" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L62" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M62" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K62" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -4693,7 +4399,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C63" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D63" s="5" t="n">
         <v>304.075925925926</v>
@@ -4702,31 +4408,24 @@
         <v>3</v>
       </c>
       <c r="F63" s="5" t="n">
-        <v>264112.0071307517</v>
+        <v>106060.9466368084</v>
       </c>
       <c r="G63" s="5" t="n">
         <v>659215.5530163825</v>
       </c>
       <c r="H63" s="5" t="n">
-        <v>923327.5601471341</v>
+        <v>765276.499653191</v>
       </c>
       <c r="I63" s="5" t="n">
-        <v>293.3528747755782</v>
+        <v>0</v>
       </c>
       <c r="J63" s="5" t="n">
-        <v>308.2395806094809</v>
-      </c>
-      <c r="K63" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L63" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M63" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N63" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K63" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -4737,7 +4436,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C64" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D64" s="5" t="n">
         <v>304.075925925926</v>
@@ -4746,31 +4445,24 @@
         <v>4</v>
       </c>
       <c r="F64" s="5" t="n">
-        <v>366716.8923585998</v>
+        <v>147264.5684450332</v>
       </c>
       <c r="G64" s="5" t="n">
         <v>878954.0706885101</v>
       </c>
       <c r="H64" s="5" t="n">
-        <v>1245670.96304711</v>
+        <v>1026218.639133543</v>
       </c>
       <c r="I64" s="5" t="n">
-        <v>294.9019811822525</v>
+        <v>0</v>
       </c>
       <c r="J64" s="5" t="n">
-        <v>309.6931564336268</v>
-      </c>
-      <c r="K64" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L64" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M64" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N64" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K64" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -4781,7 +4473,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C65" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D65" s="5" t="n">
         <v>313.15</v>
@@ -4790,31 +4482,24 @@
         <v>1</v>
       </c>
       <c r="F65" s="5" t="n">
-        <v>143196.0527859834</v>
+        <v>57504.04564385079</v>
       </c>
       <c r="G65" s="5" t="n">
         <v>214471.2781323333</v>
       </c>
       <c r="H65" s="5" t="n">
-        <v>357667.3309183166</v>
+        <v>271975.3237761841</v>
       </c>
       <c r="I65" s="5" t="n">
-        <v>290.2175291254244</v>
+        <v>0</v>
       </c>
       <c r="J65" s="5" t="n">
-        <v>314.768077611452</v>
-      </c>
-      <c r="K65" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L65" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M65" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N65" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K65" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -4825,7 +4510,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C66" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D66" s="5" t="n">
         <v>313.15</v>
@@ -4834,31 +4519,24 @@
         <v>2</v>
       </c>
       <c r="F66" s="5" t="n">
-        <v>189807.1970337624</v>
+        <v>76221.94543360507</v>
       </c>
       <c r="G66" s="5" t="n">
         <v>428942.5562646665</v>
       </c>
       <c r="H66" s="5" t="n">
-        <v>618749.753298429</v>
+        <v>505164.5016982716</v>
       </c>
       <c r="I66" s="5" t="n">
-        <v>291.7295026952932</v>
+        <v>0</v>
       </c>
       <c r="J66" s="5" t="n">
-        <v>315.949207633342</v>
-      </c>
-      <c r="K66" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L66" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M66" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K66" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -4869,7 +4547,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C67" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D67" s="5" t="n">
         <v>313.15</v>
@@ -4878,31 +4556,24 @@
         <v>3</v>
       </c>
       <c r="F67" s="5" t="n">
-        <v>264488.3059425146</v>
+        <v>106212.0590706106</v>
       </c>
       <c r="G67" s="5" t="n">
         <v>643413.8343969998</v>
       </c>
       <c r="H67" s="5" t="n">
-        <v>907902.1403395145</v>
+        <v>749625.8934676104</v>
       </c>
       <c r="I67" s="5" t="n">
-        <v>293.241476265162</v>
+        <v>0</v>
       </c>
       <c r="J67" s="5" t="n">
-        <v>317.2573254381406</v>
-      </c>
-      <c r="K67" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L67" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M67" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N67" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K67" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -4913,7 +4584,7 @@
         <v>288.7055555555556</v>
       </c>
       <c r="C68" s="5" t="n">
-        <v>0.05330378744727701</v>
+        <v>0.04342396574867613</v>
       </c>
       <c r="D68" s="5" t="n">
         <v>313.15</v>
@@ -4922,31 +4593,24 @@
         <v>4</v>
       </c>
       <c r="F68" s="5" t="n">
-        <v>367239.3795122401</v>
+        <v>147474.3865548673</v>
       </c>
       <c r="G68" s="5" t="n">
         <v>857885.1125293331</v>
       </c>
       <c r="H68" s="5" t="n">
-        <v>1225124.492041573</v>
+        <v>1005359.4990842</v>
       </c>
       <c r="I68" s="5" t="n">
-        <v>294.7534498350308</v>
+        <v>0</v>
       </c>
       <c r="J68" s="5" t="n">
-        <v>318.692431025848</v>
-      </c>
-      <c r="K68" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="L68" s="5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M68" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N68" s="5" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K68" s="5" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -5129,4 +4793,450 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="anysvml"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AZ8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13" customWidth="1" style="1" min="3" max="3"/>
+    <col width="13" customWidth="1" style="1" min="4" max="4"/>
+    <col width="13" customWidth="1" style="1" min="5" max="5"/>
+    <col width="13" customWidth="1" style="1" min="6" max="6"/>
+    <col width="13" customWidth="1" style="1" min="7" max="7"/>
+    <col width="13" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13" customWidth="1" style="1" min="9" max="9"/>
+    <col width="13" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13" customWidth="1" style="1" min="11" max="11"/>
+    <col width="13" customWidth="1" style="1" min="12" max="12"/>
+    <col width="13" customWidth="1" style="1" min="13" max="13"/>
+    <col width="13" customWidth="1" style="1" min="14" max="14"/>
+    <col width="13" customWidth="1" style="1" min="15" max="15"/>
+    <col width="13" customWidth="1" style="1" min="16" max="16"/>
+    <col width="13" customWidth="1" style="1" min="17" max="17"/>
+    <col width="13" customWidth="1" style="1" min="18" max="18"/>
+    <col width="13" customWidth="1" style="1" min="19" max="19"/>
+    <col width="13" customWidth="1" style="1" min="20" max="20"/>
+    <col width="13" customWidth="1" style="1" min="21" max="21"/>
+    <col width="13" customWidth="1" style="1" min="22" max="22"/>
+    <col width="13" customWidth="1" style="1" min="23" max="23"/>
+    <col width="13" customWidth="1" style="1" min="24" max="24"/>
+    <col width="13" customWidth="1" style="1" min="25" max="25"/>
+    <col width="13" customWidth="1" style="1" min="26" max="26"/>
+    <col width="13" customWidth="1" style="1" min="27" max="27"/>
+    <col width="13" customWidth="1" style="1" min="28" max="28"/>
+    <col width="13" customWidth="1" style="1" min="29" max="29"/>
+    <col width="13" customWidth="1" style="1" min="30" max="30"/>
+    <col width="13" customWidth="1" style="1" min="31" max="31"/>
+    <col width="13" customWidth="1" style="1" min="32" max="32"/>
+    <col width="13" customWidth="1" style="1" min="33" max="33"/>
+    <col width="13" customWidth="1" style="1" min="34" max="34"/>
+    <col width="13" customWidth="1" style="1" min="35" max="35"/>
+    <col width="13" customWidth="1" style="1" min="36" max="36"/>
+    <col width="13" customWidth="1" style="1" min="37" max="37"/>
+    <col width="13" customWidth="1" style="1" min="38" max="38"/>
+    <col width="13" customWidth="1" style="1" min="39" max="39"/>
+    <col width="13" customWidth="1" style="1" min="40" max="40"/>
+    <col width="13" customWidth="1" style="1" min="41" max="41"/>
+    <col width="13" customWidth="1" style="1" min="42" max="42"/>
+    <col width="13" customWidth="1" style="1" min="43" max="43"/>
+    <col width="13" customWidth="1" style="1" min="44" max="44"/>
+    <col width="13" customWidth="1" style="1" min="45" max="45"/>
+    <col width="13" customWidth="1" style="1" min="46" max="46"/>
+    <col width="13" customWidth="1" style="1" min="47" max="47"/>
+    <col width="13" customWidth="1" style="1" min="48" max="48"/>
+    <col width="13" customWidth="1" style="1" min="49" max="49"/>
+    <col width="13" customWidth="1" style="1" min="50" max="50"/>
+    <col width="13" customWidth="1" style="1" min="51" max="51"/>
+    <col width="13" customWidth="1" style="1" min="52" max="52"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>performance.performance_map_evaporator_liquid_pressure_differential</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="2" t="n"/>
+      <c r="AH1" s="2" t="n"/>
+      <c r="AI1" s="2" t="n"/>
+      <c r="AJ1" s="2" t="n"/>
+      <c r="AK1" s="2" t="n"/>
+      <c r="AL1" s="2" t="n"/>
+      <c r="AM1" s="2" t="n"/>
+      <c r="AN1" s="2" t="n"/>
+      <c r="AO1" s="2" t="n"/>
+      <c r="AP1" s="2" t="n"/>
+      <c r="AQ1" s="2" t="n"/>
+      <c r="AR1" s="2" t="n"/>
+      <c r="AS1" s="2" t="n"/>
+      <c r="AT1" s="2" t="n"/>
+      <c r="AU1" s="2" t="n"/>
+      <c r="AV1" s="2" t="n"/>
+      <c r="AW1" s="2" t="n"/>
+      <c r="AX1" s="2" t="n"/>
+      <c r="AY1" s="2" t="n"/>
+      <c r="AZ1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>grid_variables</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="n"/>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>lookup_variables</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>evaporator_liquid_volumetric_flow_rate</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>evaporator_liquid_leaving_temperature</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>evaporator_liquid_differential_pressure</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>m3/s</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>0.03390460960124702</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>277.0388888888889</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>0.03390460960124702</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>280.9277777777778</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>0.03390460960124702</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>284.8166666666667</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>0.03390460960124702</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>288.7055555555556</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="anysvml"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AZ8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13" customWidth="1" style="1" min="3" max="3"/>
+    <col width="13" customWidth="1" style="1" min="4" max="4"/>
+    <col width="13" customWidth="1" style="1" min="5" max="5"/>
+    <col width="13" customWidth="1" style="1" min="6" max="6"/>
+    <col width="13" customWidth="1" style="1" min="7" max="7"/>
+    <col width="13" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13" customWidth="1" style="1" min="9" max="9"/>
+    <col width="13" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13" customWidth="1" style="1" min="11" max="11"/>
+    <col width="13" customWidth="1" style="1" min="12" max="12"/>
+    <col width="13" customWidth="1" style="1" min="13" max="13"/>
+    <col width="13" customWidth="1" style="1" min="14" max="14"/>
+    <col width="13" customWidth="1" style="1" min="15" max="15"/>
+    <col width="13" customWidth="1" style="1" min="16" max="16"/>
+    <col width="13" customWidth="1" style="1" min="17" max="17"/>
+    <col width="13" customWidth="1" style="1" min="18" max="18"/>
+    <col width="13" customWidth="1" style="1" min="19" max="19"/>
+    <col width="13" customWidth="1" style="1" min="20" max="20"/>
+    <col width="13" customWidth="1" style="1" min="21" max="21"/>
+    <col width="13" customWidth="1" style="1" min="22" max="22"/>
+    <col width="13" customWidth="1" style="1" min="23" max="23"/>
+    <col width="13" customWidth="1" style="1" min="24" max="24"/>
+    <col width="13" customWidth="1" style="1" min="25" max="25"/>
+    <col width="13" customWidth="1" style="1" min="26" max="26"/>
+    <col width="13" customWidth="1" style="1" min="27" max="27"/>
+    <col width="13" customWidth="1" style="1" min="28" max="28"/>
+    <col width="13" customWidth="1" style="1" min="29" max="29"/>
+    <col width="13" customWidth="1" style="1" min="30" max="30"/>
+    <col width="13" customWidth="1" style="1" min="31" max="31"/>
+    <col width="13" customWidth="1" style="1" min="32" max="32"/>
+    <col width="13" customWidth="1" style="1" min="33" max="33"/>
+    <col width="13" customWidth="1" style="1" min="34" max="34"/>
+    <col width="13" customWidth="1" style="1" min="35" max="35"/>
+    <col width="13" customWidth="1" style="1" min="36" max="36"/>
+    <col width="13" customWidth="1" style="1" min="37" max="37"/>
+    <col width="13" customWidth="1" style="1" min="38" max="38"/>
+    <col width="13" customWidth="1" style="1" min="39" max="39"/>
+    <col width="13" customWidth="1" style="1" min="40" max="40"/>
+    <col width="13" customWidth="1" style="1" min="41" max="41"/>
+    <col width="13" customWidth="1" style="1" min="42" max="42"/>
+    <col width="13" customWidth="1" style="1" min="43" max="43"/>
+    <col width="13" customWidth="1" style="1" min="44" max="44"/>
+    <col width="13" customWidth="1" style="1" min="45" max="45"/>
+    <col width="13" customWidth="1" style="1" min="46" max="46"/>
+    <col width="13" customWidth="1" style="1" min="47" max="47"/>
+    <col width="13" customWidth="1" style="1" min="48" max="48"/>
+    <col width="13" customWidth="1" style="1" min="49" max="49"/>
+    <col width="13" customWidth="1" style="1" min="50" max="50"/>
+    <col width="13" customWidth="1" style="1" min="51" max="51"/>
+    <col width="13" customWidth="1" style="1" min="52" max="52"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>performance.performance_map_condenser_liquid_pressure_differential</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="2" t="n"/>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="P1" s="2" t="n"/>
+      <c r="Q1" s="2" t="n"/>
+      <c r="R1" s="2" t="n"/>
+      <c r="S1" s="2" t="n"/>
+      <c r="T1" s="2" t="n"/>
+      <c r="U1" s="2" t="n"/>
+      <c r="V1" s="2" t="n"/>
+      <c r="W1" s="2" t="n"/>
+      <c r="X1" s="2" t="n"/>
+      <c r="Y1" s="2" t="n"/>
+      <c r="Z1" s="2" t="n"/>
+      <c r="AA1" s="2" t="n"/>
+      <c r="AB1" s="2" t="n"/>
+      <c r="AC1" s="2" t="n"/>
+      <c r="AD1" s="2" t="n"/>
+      <c r="AE1" s="2" t="n"/>
+      <c r="AF1" s="2" t="n"/>
+      <c r="AG1" s="2" t="n"/>
+      <c r="AH1" s="2" t="n"/>
+      <c r="AI1" s="2" t="n"/>
+      <c r="AJ1" s="2" t="n"/>
+      <c r="AK1" s="2" t="n"/>
+      <c r="AL1" s="2" t="n"/>
+      <c r="AM1" s="2" t="n"/>
+      <c r="AN1" s="2" t="n"/>
+      <c r="AO1" s="2" t="n"/>
+      <c r="AP1" s="2" t="n"/>
+      <c r="AQ1" s="2" t="n"/>
+      <c r="AR1" s="2" t="n"/>
+      <c r="AS1" s="2" t="n"/>
+      <c r="AT1" s="2" t="n"/>
+      <c r="AU1" s="2" t="n"/>
+      <c r="AV1" s="2" t="n"/>
+      <c r="AW1" s="2" t="n"/>
+      <c r="AX1" s="2" t="n"/>
+      <c r="AY1" s="2" t="n"/>
+      <c r="AZ1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>grid_variables</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="n"/>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>lookup_variables</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>condenser_liquid_volumetric_flow_rate</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>condenser_liquid_entering_temperature</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>condenser_liquid_differential_pressure</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>m3/s</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>0.04342396574867613</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>285.9277777777778</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>0.04342396574867613</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>295.0018518518519</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>0.04342396574867613</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>304.075925925926</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>0.04342396574867613</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>313.15</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="anysvml"/>
+</worksheet>
 </file>
</xml_diff>